<commit_message>
Updated CD3 templates with standard groups and policies
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-mvt-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-mvt-template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22990" windowHeight="8280"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22990" windowHeight="8280" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="1" r:id="rId1"/>
@@ -5945,9 +5945,6 @@
     <t>Database Operations</t>
   </si>
   <si>
-    <t>Netwok_Ops</t>
-  </si>
-  <si>
     <t>Network Operations</t>
   </si>
   <si>
@@ -6144,6 +6141,9 @@
   </si>
   <si>
     <t>Allow group Database_Ops to use database-family in tenancy</t>
+  </si>
+  <si>
+    <t>Network_Ops</t>
   </si>
 </sst>
 </file>
@@ -7302,7 +7302,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+    <sheetView zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -12766,8 +12766,8 @@
   </sheetPr>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12954,10 +12954,10 @@
         <v>321</v>
       </c>
       <c r="B15" s="56" t="s">
+        <v>718</v>
+      </c>
+      <c r="C15" s="45" t="s">
         <v>652</v>
-      </c>
-      <c r="C15" s="45" t="s">
-        <v>653</v>
       </c>
     </row>
   </sheetData>
@@ -13034,16 +13034,16 @@
         <v>321</v>
       </c>
       <c r="B3" s="45" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C3" s="45" t="s">
         <v>389</v>
       </c>
       <c r="D3" s="45" t="s">
+        <v>654</v>
+      </c>
+      <c r="E3" s="93" t="s">
         <v>655</v>
-      </c>
-      <c r="E3" s="93" t="s">
-        <v>656</v>
       </c>
       <c r="F3" s="45"/>
       <c r="G3" s="45"/>
@@ -13054,16 +13054,16 @@
         <v>321</v>
       </c>
       <c r="B4" s="45" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C4" s="47" t="s">
         <v>389</v>
       </c>
       <c r="D4" s="45" t="s">
+        <v>657</v>
+      </c>
+      <c r="E4" s="45" t="s">
         <v>658</v>
-      </c>
-      <c r="E4" s="45" t="s">
-        <v>659</v>
       </c>
       <c r="F4" s="47"/>
       <c r="G4" s="47"/>
@@ -13073,16 +13073,16 @@
         <v>321</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C5" s="47" t="s">
         <v>389</v>
       </c>
       <c r="D5" s="45" t="s">
+        <v>660</v>
+      </c>
+      <c r="E5" s="45" t="s">
         <v>661</v>
-      </c>
-      <c r="E5" s="45" t="s">
-        <v>662</v>
       </c>
       <c r="F5" s="47"/>
       <c r="G5" s="47"/>
@@ -13093,7 +13093,7 @@
       <c r="C6" s="47"/>
       <c r="D6" s="45"/>
       <c r="E6" s="45" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="F6" s="47"/>
       <c r="G6" s="47"/>
@@ -13104,7 +13104,7 @@
       <c r="C7" s="47"/>
       <c r="D7" s="45"/>
       <c r="E7" s="45" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F7" s="47"/>
       <c r="G7" s="47"/>
@@ -13115,7 +13115,7 @@
       <c r="C8" s="47"/>
       <c r="D8" s="45"/>
       <c r="E8" s="45" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F8" s="47"/>
       <c r="G8" s="47"/>
@@ -13126,7 +13126,7 @@
       <c r="C9" s="47"/>
       <c r="D9" s="45"/>
       <c r="E9" s="45" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="F9" s="47"/>
       <c r="G9" s="47"/>
@@ -13137,7 +13137,7 @@
       <c r="C10" s="47"/>
       <c r="D10" s="45"/>
       <c r="E10" s="45" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="F10" s="47"/>
       <c r="G10" s="47"/>
@@ -13148,7 +13148,7 @@
       <c r="C11" s="47"/>
       <c r="D11" s="45"/>
       <c r="E11" s="45" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="F11" s="47"/>
       <c r="G11" s="47"/>
@@ -13158,16 +13158,16 @@
         <v>321</v>
       </c>
       <c r="B12" s="45" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C12" s="47" t="s">
         <v>389</v>
       </c>
       <c r="D12" s="45" t="s">
+        <v>669</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>670</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>671</v>
       </c>
       <c r="F12" s="47"/>
       <c r="G12" s="47"/>
@@ -13177,16 +13177,16 @@
         <v>321</v>
       </c>
       <c r="B13" s="45" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C13" s="47" t="s">
         <v>389</v>
       </c>
       <c r="D13" s="45" t="s">
+        <v>672</v>
+      </c>
+      <c r="E13" s="45" t="s">
         <v>673</v>
-      </c>
-      <c r="E13" s="45" t="s">
-        <v>674</v>
       </c>
       <c r="F13" s="47"/>
       <c r="G13" s="47"/>
@@ -13197,7 +13197,7 @@
       <c r="C14" s="47"/>
       <c r="D14" s="45"/>
       <c r="E14" s="45" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="F14" s="47"/>
       <c r="G14" s="47"/>
@@ -13208,7 +13208,7 @@
       <c r="C15" s="47"/>
       <c r="D15" s="45"/>
       <c r="E15" s="45" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="F15" s="47"/>
       <c r="G15" s="47"/>
@@ -13219,7 +13219,7 @@
       <c r="C16" s="47"/>
       <c r="D16" s="45"/>
       <c r="E16" s="45" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="F16" s="47"/>
       <c r="G16" s="47"/>
@@ -13229,16 +13229,16 @@
         <v>321</v>
       </c>
       <c r="B17" s="45" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C17" s="47" t="s">
         <v>389</v>
       </c>
       <c r="D17" s="45" t="s">
+        <v>678</v>
+      </c>
+      <c r="E17" s="45" t="s">
         <v>679</v>
-      </c>
-      <c r="E17" s="45" t="s">
-        <v>680</v>
       </c>
       <c r="F17" s="47"/>
       <c r="G17" s="47"/>
@@ -13249,7 +13249,7 @@
       <c r="C18" s="47"/>
       <c r="D18" s="45"/>
       <c r="E18" s="45" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="F18" s="47"/>
       <c r="G18" s="47"/>
@@ -13260,7 +13260,7 @@
       <c r="C19" s="47"/>
       <c r="D19" s="45"/>
       <c r="E19" s="45" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="F19" s="47"/>
       <c r="G19" s="47"/>
@@ -13271,7 +13271,7 @@
       <c r="C20" s="47"/>
       <c r="D20" s="45"/>
       <c r="E20" s="45" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="F20" s="47"/>
       <c r="G20" s="47"/>
@@ -13282,7 +13282,7 @@
       <c r="C21" s="47"/>
       <c r="D21" s="45"/>
       <c r="E21" s="45" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="F21" s="47"/>
       <c r="G21" s="47"/>
@@ -13293,7 +13293,7 @@
       <c r="C22" s="47"/>
       <c r="D22" s="45"/>
       <c r="E22" s="45" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="F22" s="47"/>
       <c r="G22" s="47"/>
@@ -13304,7 +13304,7 @@
       <c r="C23" s="47"/>
       <c r="D23" s="45"/>
       <c r="E23" s="45" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="F23" s="47"/>
       <c r="G23" s="47"/>
@@ -13315,7 +13315,7 @@
       <c r="C24" s="47"/>
       <c r="D24" s="45"/>
       <c r="E24" s="45" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="F24" s="47"/>
       <c r="G24" s="47"/>
@@ -13326,7 +13326,7 @@
       <c r="C25" s="47"/>
       <c r="D25" s="45"/>
       <c r="E25" s="45" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="F25" s="47"/>
       <c r="G25" s="47"/>
@@ -13336,16 +13336,16 @@
         <v>321</v>
       </c>
       <c r="B26" s="45" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C26" s="47" t="s">
         <v>389</v>
       </c>
       <c r="D26" s="45" t="s">
+        <v>689</v>
+      </c>
+      <c r="E26" s="45" t="s">
         <v>690</v>
-      </c>
-      <c r="E26" s="45" t="s">
-        <v>691</v>
       </c>
       <c r="F26" s="47"/>
       <c r="G26" s="47"/>
@@ -13356,7 +13356,7 @@
       <c r="C27" s="47"/>
       <c r="D27" s="45"/>
       <c r="E27" s="45" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="F27" s="47"/>
       <c r="G27" s="47"/>
@@ -13367,7 +13367,7 @@
       <c r="C28" s="47"/>
       <c r="D28" s="45"/>
       <c r="E28" s="45" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F28" s="47"/>
       <c r="G28" s="47"/>
@@ -13378,7 +13378,7 @@
       <c r="C29" s="47"/>
       <c r="D29" s="45"/>
       <c r="E29" s="45" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="F29" s="47"/>
       <c r="G29" s="47"/>
@@ -13388,16 +13388,16 @@
         <v>321</v>
       </c>
       <c r="B30" s="45" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C30" s="47" t="s">
         <v>389</v>
       </c>
       <c r="D30" s="45" t="s">
+        <v>695</v>
+      </c>
+      <c r="E30" s="45" t="s">
         <v>696</v>
-      </c>
-      <c r="E30" s="45" t="s">
-        <v>697</v>
       </c>
       <c r="F30" s="47"/>
       <c r="G30" s="47"/>
@@ -13408,7 +13408,7 @@
       <c r="C31" s="47"/>
       <c r="D31" s="45"/>
       <c r="E31" s="45" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="F31" s="47"/>
       <c r="G31" s="47"/>
@@ -13419,7 +13419,7 @@
       <c r="C32" s="47"/>
       <c r="D32" s="45"/>
       <c r="E32" s="45" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="F32" s="47"/>
       <c r="G32" s="47"/>
@@ -13430,7 +13430,7 @@
       <c r="C33" s="47"/>
       <c r="D33" s="45"/>
       <c r="E33" s="45" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="F33" s="47"/>
       <c r="G33" s="47"/>
@@ -13441,7 +13441,7 @@
       <c r="C34" s="47"/>
       <c r="D34" s="45"/>
       <c r="E34" s="45" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="F34" s="47"/>
       <c r="G34" s="47"/>
@@ -13452,7 +13452,7 @@
       <c r="C35" s="47"/>
       <c r="D35" s="45"/>
       <c r="E35" s="45" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="F35" s="47"/>
       <c r="G35" s="47"/>
@@ -13462,16 +13462,16 @@
         <v>321</v>
       </c>
       <c r="B36" s="45" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C36" s="47" t="s">
         <v>389</v>
       </c>
       <c r="D36" s="45" t="s">
+        <v>702</v>
+      </c>
+      <c r="E36" s="45" t="s">
         <v>703</v>
-      </c>
-      <c r="E36" s="45" t="s">
-        <v>704</v>
       </c>
       <c r="F36" s="47"/>
       <c r="G36" s="47"/>
@@ -13482,7 +13482,7 @@
       <c r="C37" s="47"/>
       <c r="D37" s="45"/>
       <c r="E37" s="45" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="F37" s="47"/>
       <c r="G37" s="47"/>
@@ -13493,7 +13493,7 @@
       <c r="C38" s="47"/>
       <c r="D38" s="45"/>
       <c r="E38" s="45" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="F38" s="47"/>
       <c r="G38" s="47"/>
@@ -13504,7 +13504,7 @@
       <c r="C39" s="47"/>
       <c r="D39" s="45"/>
       <c r="E39" s="45" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="F39" s="47"/>
       <c r="G39" s="47"/>
@@ -13515,7 +13515,7 @@
       <c r="C40" s="47"/>
       <c r="D40" s="45"/>
       <c r="E40" s="45" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="F40" s="47"/>
       <c r="G40" s="47"/>
@@ -13525,16 +13525,16 @@
         <v>321</v>
       </c>
       <c r="B41" s="45" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C41" s="47" t="s">
         <v>389</v>
       </c>
       <c r="D41" s="45" t="s">
+        <v>709</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>710</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>711</v>
       </c>
       <c r="F41" s="47"/>
       <c r="G41" s="47"/>
@@ -13544,16 +13544,16 @@
         <v>321</v>
       </c>
       <c r="B42" s="45" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="C42" s="47" t="s">
         <v>389</v>
       </c>
       <c r="D42" s="45" t="s">
+        <v>712</v>
+      </c>
+      <c r="E42" s="45" t="s">
         <v>713</v>
-      </c>
-      <c r="E42" s="45" t="s">
-        <v>714</v>
       </c>
       <c r="F42" s="47"/>
       <c r="G42" s="47"/>
@@ -13564,7 +13564,7 @@
       <c r="C43" s="47"/>
       <c r="D43" s="45"/>
       <c r="E43" s="45" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="F43" s="47"/>
       <c r="G43" s="47"/>
@@ -13574,16 +13574,16 @@
         <v>321</v>
       </c>
       <c r="B44" s="45" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C44" s="47" t="s">
         <v>389</v>
       </c>
       <c r="D44" s="45" t="s">
+        <v>716</v>
+      </c>
+      <c r="E44" s="45" t="s">
         <v>717</v>
-      </c>
-      <c r="E44" s="45" t="s">
-        <v>718</v>
       </c>
       <c r="F44" s="47"/>
       <c r="G44" s="47"/>
@@ -13887,7 +13887,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Clean up of CD3 borders
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-mvt-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-mvt-template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\oci_develop\oci_tenancy\SetUpOCI_Via_TF\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CD3aaS\code\oci_tenancy\SetUpOCI_Via_TF\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22990" windowHeight="8280" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22992" windowHeight="8280"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="719">
   <si>
     <t>Region</t>
   </si>
@@ -6631,7 +6631,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -6849,6 +6849,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -7302,17 +7303,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="167.08984375" style="46" customWidth="1"/>
+    <col min="1" max="1" width="167.109375" style="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="1:1" ht="59" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:1" ht="58.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="88" t="s">
         <v>489</v>
       </c>
@@ -7334,49 +7335,49 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="46" customWidth="1"/>
-    <col min="2" max="2" width="26.81640625" style="46" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.81640625" style="46" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.81640625" style="46" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.1796875" style="46" customWidth="1"/>
-    <col min="6" max="6" width="24.1796875" style="46" customWidth="1"/>
-    <col min="7" max="7" width="18.1796875" style="46" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.81640625" style="46" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.81640625" style="46" customWidth="1"/>
-    <col min="10" max="10" width="22.08984375" style="46" customWidth="1"/>
-    <col min="11" max="11" width="26.81640625" style="46" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" style="46" customWidth="1"/>
+    <col min="2" max="2" width="26.77734375" style="46" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" style="46" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" style="46" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.21875" style="46" customWidth="1"/>
+    <col min="6" max="6" width="24.21875" style="46" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" style="46" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.77734375" style="46" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.77734375" style="46" customWidth="1"/>
+    <col min="10" max="10" width="22.109375" style="46" customWidth="1"/>
+    <col min="11" max="11" width="26.77734375" style="46" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" style="46" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19" style="46" customWidth="1"/>
-    <col min="14" max="14" width="19.1796875" style="46" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.36328125" style="46" customWidth="1"/>
-    <col min="16" max="16" width="12.81640625" customWidth="1"/>
+    <col min="14" max="14" width="19.21875" style="46" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.33203125" style="46" customWidth="1"/>
+    <col min="16" max="16" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="117" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="103" t="s">
+    <row r="1" spans="1:16" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="104" t="s">
         <v>488</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="96" t="s">
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="106"/>
+      <c r="I1" s="97" t="s">
         <v>598</v>
       </c>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
-      <c r="M1" s="97"/>
-      <c r="N1" s="97"/>
-      <c r="O1" s="97"/>
-      <c r="P1" s="98"/>
-    </row>
-    <row r="2" spans="1:16" s="54" customFormat="1" ht="52.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="98"/>
+      <c r="O1" s="98"/>
+      <c r="P1" s="99"/>
+    </row>
+    <row r="2" spans="1:16" s="54" customFormat="1" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
         <v>0</v>
       </c>
@@ -7426,7 +7427,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="46" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" s="46" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>321</v>
       </c>
@@ -7464,7 +7465,7 @@
       <c r="O3" s="47"/>
       <c r="P3" s="47"/>
     </row>
-    <row r="4" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
         <v>321</v>
       </c>
@@ -7502,7 +7503,7 @@
       <c r="O4" s="47"/>
       <c r="P4" s="47"/>
     </row>
-    <row r="5" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="56" t="s">
         <v>321</v>
       </c>
@@ -7540,7 +7541,7 @@
       <c r="O5" s="47"/>
       <c r="P5" s="47"/>
     </row>
-    <row r="6" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="56" t="s">
         <v>321</v>
       </c>
@@ -7578,7 +7579,7 @@
       <c r="O6" s="47"/>
       <c r="P6" s="47"/>
     </row>
-    <row r="7" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="56" t="s">
         <v>321</v>
       </c>
@@ -7616,7 +7617,7 @@
       <c r="O7" s="47"/>
       <c r="P7" s="47"/>
     </row>
-    <row r="8" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="56" t="s">
         <v>4</v>
       </c>
@@ -7657,34 +7658,34 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="46" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" style="46" customWidth="1"/>
     <col min="2" max="2" width="23" style="46" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" style="46" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" style="46" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.81640625" style="46" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.1796875" style="46" customWidth="1"/>
-    <col min="7" max="7" width="26.81640625" style="46" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.453125" style="46" customWidth="1"/>
-    <col min="10" max="10" width="14.54296875" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" style="46" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" style="46" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.77734375" style="46" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.21875" style="46" customWidth="1"/>
+    <col min="7" max="7" width="26.77734375" style="46" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" style="46" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="114.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="96" t="s">
+    <row r="1" spans="1:10" ht="114.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="97" t="s">
         <v>599</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="98"/>
-    </row>
-    <row r="2" spans="1:10" s="54" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="99"/>
+    </row>
+    <row r="2" spans="1:10" s="54" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -7716,7 +7717,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>321</v>
       </c>
@@ -7742,7 +7743,7 @@
       <c r="I3" s="47"/>
       <c r="J3" s="47"/>
     </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
         <v>321</v>
       </c>
@@ -7768,7 +7769,7 @@
       <c r="I4" s="47"/>
       <c r="J4" s="45"/>
     </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
         <v>321</v>
       </c>
@@ -7794,7 +7795,7 @@
       <c r="I5" s="47"/>
       <c r="J5" s="47"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>321</v>
       </c>
@@ -7820,7 +7821,7 @@
       <c r="I6" s="47"/>
       <c r="J6" s="47"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
         <v>321</v>
       </c>
@@ -7846,7 +7847,7 @@
       <c r="I7" s="47"/>
       <c r="J7" s="47"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="56" t="s">
         <v>4</v>
       </c>
@@ -7880,33 +7881,33 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="46" customWidth="1"/>
-    <col min="2" max="2" width="19.1796875" style="46" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.54296875" style="46" customWidth="1"/>
-    <col min="4" max="4" width="25.08984375" style="46" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" style="46" customWidth="1"/>
+    <col min="2" max="2" width="19.21875" style="46" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" style="46" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" style="46" customWidth="1"/>
     <col min="5" max="5" width="16" style="46" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.81640625" style="46" customWidth="1"/>
-    <col min="7" max="7" width="16.1796875" style="46" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.1796875" style="46" customWidth="1"/>
-    <col min="9" max="9" width="12.36328125" customWidth="1"/>
+    <col min="6" max="6" width="31.77734375" style="46" customWidth="1"/>
+    <col min="7" max="7" width="16.21875" style="46" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" style="46" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="95" t="s">
+    <row r="1" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="96" t="s">
         <v>462</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -7955,40 +7956,40 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="46" customWidth="1"/>
-    <col min="2" max="2" width="17.81640625" style="46" customWidth="1"/>
-    <col min="3" max="3" width="14.90625" style="46" customWidth="1"/>
-    <col min="4" max="4" width="33.08984375" style="46" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" style="46" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.1796875" style="46" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.08984375" style="46" customWidth="1"/>
-    <col min="17" max="17" width="11.6328125" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" style="46" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" style="46" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" style="46" customWidth="1"/>
+    <col min="4" max="4" width="33.109375" style="46" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" style="46" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.21875" style="46" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.109375" style="46" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="95" t="s">
+    <row r="1" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="96" t="s">
         <v>463</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="95"/>
-      <c r="P1" s="95"/>
-      <c r="Q1" s="95"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="96"/>
+      <c r="O1" s="96"/>
+      <c r="P1" s="96"/>
+      <c r="Q1" s="96"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -8057,48 +8058,48 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.453125" style="46" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.08984375" style="46" customWidth="1"/>
-    <col min="3" max="3" width="17.1796875" style="46" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" style="46" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" style="46" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" style="46" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1796875" style="46" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.81640625" style="46" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" style="46" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" style="46" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" style="46" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" style="46" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" style="46" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.21875" style="46" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.21875" style="46" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.77734375" style="46" customWidth="1"/>
     <col min="11" max="11" width="19" style="46" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1796875" style="46" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.08984375" style="46" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.21875" style="46" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.109375" style="46" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="118.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="95" t="s">
+    <row r="1" spans="1:20" ht="118.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="96" t="s">
         <v>470</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="95"/>
-      <c r="P1" s="95"/>
-      <c r="Q1" s="95"/>
-      <c r="R1" s="95"/>
-      <c r="S1" s="95"/>
-      <c r="T1" s="95"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="96"/>
+      <c r="O1" s="96"/>
+      <c r="P1" s="96"/>
+      <c r="Q1" s="96"/>
+      <c r="R1" s="96"/>
+      <c r="S1" s="96"/>
+      <c r="T1" s="96"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -8160,7 +8161,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>4</v>
       </c>
@@ -8184,7 +8185,7 @@
       <c r="S3" s="47"/>
       <c r="T3" s="47"/>
     </row>
-    <row r="4" spans="1:20" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
         <v>5</v>
       </c>
@@ -8226,7 +8227,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
         <v>5</v>
       </c>
@@ -8270,7 +8271,7 @@
       <c r="S5" s="47"/>
       <c r="T5" s="47"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>5</v>
       </c>
@@ -8308,7 +8309,7 @@
       <c r="S6" s="47"/>
       <c r="T6" s="47"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
         <v>5</v>
       </c>
@@ -8369,28 +8370,28 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.1796875" style="46" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.21875" style="46" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="46" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" style="46" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" style="46" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" style="46" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" style="46" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="46" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.6328125" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="95" t="s">
+    <row r="1" spans="1:7" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="96" t="s">
         <v>471</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-    </row>
-    <row r="2" spans="1:7" s="54" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+    </row>
+    <row r="2" spans="1:7" s="54" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
         <v>0</v>
       </c>
@@ -8413,7 +8414,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>4</v>
       </c>
@@ -8424,7 +8425,7 @@
       <c r="F3" s="47"/>
       <c r="G3" s="47"/>
     </row>
-    <row r="4" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
         <v>5</v>
       </c>
@@ -8447,7 +8448,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
         <v>5</v>
       </c>
@@ -8468,7 +8469,7 @@
       </c>
       <c r="G5" s="47"/>
     </row>
-    <row r="6" spans="1:7" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>5</v>
       </c>
@@ -8505,50 +8506,50 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.453125" style="46" customWidth="1"/>
-    <col min="3" max="3" width="17.1796875" style="46" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" style="46" customWidth="1"/>
-    <col min="5" max="5" width="20.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.90625" style="46" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" style="46" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" style="46" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="46" customWidth="1"/>
+    <col min="5" max="5" width="20.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" style="46" customWidth="1"/>
     <col min="7" max="7" width="15" style="46" customWidth="1"/>
-    <col min="8" max="8" width="8.36328125" style="46" customWidth="1"/>
-    <col min="9" max="9" width="9.81640625" style="46" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="46" customWidth="1"/>
+    <col min="9" max="9" width="9.77734375" style="46" customWidth="1"/>
     <col min="10" max="10" width="16" style="46" customWidth="1"/>
-    <col min="11" max="11" width="19.1796875" style="46" customWidth="1"/>
-    <col min="12" max="12" width="7.81640625" style="46" customWidth="1"/>
-    <col min="13" max="13" width="8.453125" style="46" customWidth="1"/>
-    <col min="14" max="14" width="17.08984375" style="46" customWidth="1"/>
-    <col min="15" max="15" width="15.6328125" style="46" customWidth="1"/>
-    <col min="16" max="16" width="18.90625" customWidth="1"/>
-    <col min="17" max="17" width="12.36328125" customWidth="1"/>
+    <col min="11" max="11" width="19.21875" style="46" customWidth="1"/>
+    <col min="12" max="12" width="7.77734375" style="46" customWidth="1"/>
+    <col min="13" max="13" width="8.44140625" style="46" customWidth="1"/>
+    <col min="14" max="14" width="17.109375" style="46" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" style="46" customWidth="1"/>
+    <col min="16" max="16" width="18.88671875" customWidth="1"/>
+    <col min="17" max="17" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="110.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="106" t="s">
+    <row r="1" spans="1:17" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="107" t="s">
         <v>478</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="108"/>
-      <c r="I1" s="109" t="s">
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="110" t="s">
         <v>472</v>
       </c>
-      <c r="J1" s="109"/>
-      <c r="K1" s="109"/>
-      <c r="L1" s="109"/>
-      <c r="M1" s="109"/>
-      <c r="N1" s="109"/>
-      <c r="O1" s="109"/>
-      <c r="P1" s="109"/>
-      <c r="Q1" s="109"/>
-    </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J1" s="110"/>
+      <c r="K1" s="110"/>
+      <c r="L1" s="110"/>
+      <c r="M1" s="110"/>
+      <c r="N1" s="110"/>
+      <c r="O1" s="110"/>
+      <c r="P1" s="110"/>
+      <c r="Q1" s="110"/>
+    </row>
+    <row r="2" spans="1:17" s="1" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
@@ -8601,7 +8602,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>4</v>
       </c>
@@ -8622,7 +8623,7 @@
       <c r="P3" s="47"/>
       <c r="Q3" s="47"/>
     </row>
-    <row r="4" spans="1:17" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>5</v>
       </c>
@@ -8661,7 +8662,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="30"/>
       <c r="B5" s="47"/>
       <c r="C5" s="30"/>
@@ -8686,7 +8687,7 @@
       <c r="P5" s="47"/>
       <c r="Q5" s="47"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="30"/>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -8710,7 +8711,7 @@
       <c r="P6" s="47"/>
       <c r="Q6" s="47"/>
     </row>
-    <row r="7" spans="1:17" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="30" t="s">
         <v>5</v>
       </c>
@@ -8743,7 +8744,7 @@
       <c r="P7" s="47"/>
       <c r="Q7" s="47"/>
     </row>
-    <row r="8" spans="1:17" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="s">
         <v>5</v>
       </c>
@@ -8782,7 +8783,7 @@
       </c>
       <c r="Q8" s="47"/>
     </row>
-    <row r="9" spans="1:17" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="30" t="s">
         <v>5</v>
       </c>
@@ -8819,7 +8820,7 @@
       <c r="P9" s="47"/>
       <c r="Q9" s="47"/>
     </row>
-    <row r="10" spans="1:17" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
         <v>5</v>
       </c>
@@ -8870,41 +8871,41 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.6328125" style="46" customWidth="1"/>
-    <col min="3" max="3" width="13.6328125" style="46" customWidth="1"/>
-    <col min="4" max="4" width="16.08984375" style="46" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" style="46" customWidth="1"/>
-    <col min="6" max="6" width="18.90625" style="46" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="46" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="46" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" style="46" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" style="46" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" style="46" customWidth="1"/>
     <col min="8" max="8" width="25" style="46" customWidth="1"/>
-    <col min="9" max="9" width="31.08984375" style="46" customWidth="1"/>
-    <col min="11" max="11" width="7.453125" style="46" customWidth="1"/>
-    <col min="13" max="13" width="28.1796875" style="46" customWidth="1"/>
-    <col min="14" max="14" width="13.6328125" customWidth="1"/>
+    <col min="9" max="9" width="31.109375" style="46" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" style="46" customWidth="1"/>
+    <col min="13" max="13" width="28.21875" style="46" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="122.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="95" t="s">
+    <row r="1" spans="1:16" ht="122.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="96" t="s">
         <v>464</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="95"/>
-      <c r="P1" s="95"/>
-    </row>
-    <row r="2" spans="1:16" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="96"/>
+      <c r="O1" s="96"/>
+      <c r="P1" s="96"/>
+    </row>
+    <row r="2" spans="1:16" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
@@ -8954,7 +8955,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="45" t="s">
         <v>4</v>
       </c>
@@ -8974,7 +8975,7 @@
       <c r="O3" s="47"/>
       <c r="P3" s="47"/>
     </row>
-    <row r="4" spans="1:16" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
         <v>5</v>
       </c>
@@ -9018,7 +9019,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="37.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="47"/>
       <c r="B5" s="47"/>
       <c r="C5" s="47"/>
@@ -9042,7 +9043,7 @@
       <c r="O5" s="47"/>
       <c r="P5" s="47"/>
     </row>
-    <row r="6" spans="1:16" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>5</v>
       </c>
@@ -9103,49 +9104,49 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.1796875" style="46" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" style="46" customWidth="1"/>
     <col min="3" max="3" width="11" style="46" customWidth="1"/>
-    <col min="4" max="5" width="10.90625" style="46" customWidth="1"/>
+    <col min="4" max="5" width="10.88671875" style="46" customWidth="1"/>
     <col min="6" max="6" width="18" style="46" customWidth="1"/>
-    <col min="7" max="7" width="18.81640625" style="46" customWidth="1"/>
-    <col min="8" max="8" width="16.08984375" style="46" customWidth="1"/>
-    <col min="9" max="9" width="11.90625" style="46" customWidth="1"/>
-    <col min="10" max="11" width="14.6328125" style="46" customWidth="1"/>
-    <col min="12" max="12" width="14.36328125" style="46" customWidth="1"/>
-    <col min="14" max="14" width="23.6328125" style="46" customWidth="1"/>
-    <col min="16" max="16" width="12.6328125" style="46" customWidth="1"/>
-    <col min="17" max="17" width="14.81640625" style="46" customWidth="1"/>
-    <col min="21" max="21" width="11.453125" customWidth="1"/>
+    <col min="7" max="7" width="18.77734375" style="46" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" style="46" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" style="46" customWidth="1"/>
+    <col min="10" max="11" width="14.6640625" style="46" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" style="46" customWidth="1"/>
+    <col min="14" max="14" width="23.6640625" style="46" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" style="46" customWidth="1"/>
+    <col min="17" max="17" width="14.77734375" style="46" customWidth="1"/>
+    <col min="21" max="21" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="87.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="96" t="s">
+    <row r="1" spans="1:21" ht="87.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="97" t="s">
         <v>485</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
-      <c r="M1" s="97"/>
-      <c r="N1" s="97"/>
-      <c r="O1" s="97"/>
-      <c r="P1" s="97"/>
-      <c r="Q1" s="97"/>
-      <c r="R1" s="97"/>
-      <c r="S1" s="97"/>
-      <c r="T1" s="97"/>
-      <c r="U1" s="98"/>
-    </row>
-    <row r="2" spans="1:21" ht="58.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="98"/>
+      <c r="O1" s="98"/>
+      <c r="P1" s="98"/>
+      <c r="Q1" s="98"/>
+      <c r="R1" s="98"/>
+      <c r="S1" s="98"/>
+      <c r="T1" s="98"/>
+      <c r="U1" s="99"/>
+    </row>
+    <row r="2" spans="1:21" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="48" t="s">
         <v>0</v>
       </c>
@@ -9210,7 +9211,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>4</v>
       </c>
@@ -9235,7 +9236,7 @@
       <c r="T3" s="47"/>
       <c r="U3" s="47"/>
     </row>
-    <row r="4" spans="1:21" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
         <v>5</v>
       </c>
@@ -9298,7 +9299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="47"/>
       <c r="B5" s="47"/>
       <c r="C5" s="47"/>
@@ -9341,7 +9342,7 @@
       <c r="T5" s="47"/>
       <c r="U5" s="47"/>
     </row>
-    <row r="6" spans="1:21" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>5</v>
       </c>
@@ -9405,49 +9406,49 @@
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.81640625" style="46" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" style="46" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" style="46" customWidth="1"/>
-    <col min="6" max="6" width="17.36328125" style="46" customWidth="1"/>
-    <col min="7" max="7" width="16.453125" style="46" customWidth="1"/>
-    <col min="8" max="8" width="19.1796875" style="46" customWidth="1"/>
-    <col min="9" max="9" width="13.6328125" style="46" customWidth="1"/>
-    <col min="10" max="10" width="12.54296875" style="46" customWidth="1"/>
-    <col min="11" max="11" width="13.1796875" style="46" customWidth="1"/>
-    <col min="13" max="13" width="15.1796875" style="46" customWidth="1"/>
-    <col min="14" max="16" width="13.81640625" style="46" customWidth="1"/>
-    <col min="17" max="17" width="21.08984375" style="46" customWidth="1"/>
-    <col min="18" max="18" width="17.1796875" style="46" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" style="46" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" style="46" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" style="46" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="46" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" style="46" customWidth="1"/>
+    <col min="8" max="8" width="19.21875" style="46" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="46" customWidth="1"/>
+    <col min="10" max="10" width="12.5546875" style="46" customWidth="1"/>
+    <col min="11" max="11" width="13.21875" style="46" customWidth="1"/>
+    <col min="13" max="13" width="15.21875" style="46" customWidth="1"/>
+    <col min="14" max="16" width="13.77734375" style="46" customWidth="1"/>
+    <col min="17" max="17" width="21.109375" style="46" customWidth="1"/>
+    <col min="18" max="18" width="17.21875" style="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="115.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="96" t="s">
+    <row r="1" spans="1:19" ht="115.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="97" t="s">
         <v>455</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="99" t="s">
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="100" t="s">
         <v>481</v>
       </c>
-      <c r="K1" s="110"/>
-      <c r="L1" s="110"/>
-      <c r="M1" s="110"/>
-      <c r="N1" s="110"/>
-      <c r="O1" s="110"/>
-      <c r="P1" s="110"/>
-      <c r="Q1" s="110"/>
-      <c r="R1" s="110"/>
-      <c r="S1" s="111"/>
-    </row>
-    <row r="2" spans="1:19" ht="58.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="K1" s="111"/>
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="111"/>
+      <c r="O1" s="111"/>
+      <c r="P1" s="111"/>
+      <c r="Q1" s="111"/>
+      <c r="R1" s="111"/>
+      <c r="S1" s="112"/>
+    </row>
+    <row r="2" spans="1:19" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
@@ -9506,7 +9507,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="21.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>4</v>
       </c>
@@ -9529,7 +9530,7 @@
       <c r="R3" s="47"/>
       <c r="S3" s="47"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
         <v>5</v>
       </c>
@@ -9562,7 +9563,7 @@
       </c>
       <c r="S4" s="47"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="47"/>
       <c r="B5" s="47"/>
       <c r="C5" s="47"/>
@@ -9585,7 +9586,7 @@
       <c r="R5" s="47"/>
       <c r="S5" s="47"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="47"/>
       <c r="B6" s="47"/>
       <c r="C6" s="47"/>
@@ -9608,7 +9609,7 @@
       <c r="R6" s="47"/>
       <c r="S6" s="47"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="47"/>
       <c r="B7" s="47"/>
       <c r="C7" s="47"/>
@@ -9631,7 +9632,7 @@
       <c r="R7" s="47"/>
       <c r="S7" s="47"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="47"/>
       <c r="B8" s="47"/>
       <c r="C8" s="47"/>
@@ -9654,7 +9655,7 @@
       <c r="R8" s="47"/>
       <c r="S8" s="47"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="47"/>
       <c r="B9" s="47"/>
       <c r="C9" s="47"/>
@@ -9681,7 +9682,7 @@
       <c r="R9" s="47"/>
       <c r="S9" s="47"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="47"/>
       <c r="B10" s="47"/>
       <c r="C10" s="47"/>
@@ -9710,7 +9711,7 @@
       <c r="R10" s="47"/>
       <c r="S10" s="47"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="47"/>
       <c r="B11" s="47"/>
       <c r="C11" s="47"/>
@@ -9745,7 +9746,7 @@
       <c r="R11" s="47"/>
       <c r="S11" s="47"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="47"/>
       <c r="B12" s="47"/>
       <c r="C12" s="47"/>
@@ -9780,7 +9781,7 @@
       <c r="R12" s="47"/>
       <c r="S12" s="47"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="47"/>
       <c r="B13" s="47"/>
       <c r="C13" s="47"/>
@@ -9807,7 +9808,7 @@
       <c r="R13" s="47"/>
       <c r="S13" s="47"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="47"/>
       <c r="B14" s="47"/>
       <c r="C14" s="47"/>
@@ -9834,7 +9835,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="47"/>
       <c r="B15" s="47"/>
       <c r="C15" s="47"/>
@@ -9859,7 +9860,7 @@
       <c r="R15" s="47"/>
       <c r="S15" s="47"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="47"/>
       <c r="B16" s="47"/>
       <c r="C16" s="47"/>
@@ -9886,7 +9887,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="47"/>
       <c r="B17" s="47"/>
       <c r="C17" s="47"/>
@@ -9911,7 +9912,7 @@
       <c r="R17" s="47"/>
       <c r="S17" s="47"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="47"/>
       <c r="B18" s="47"/>
       <c r="C18" s="47"/>
@@ -9938,7 +9939,7 @@
       <c r="R18" s="47"/>
       <c r="S18" s="47"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="47"/>
       <c r="B19" s="47"/>
       <c r="C19" s="47"/>
@@ -9959,7 +9960,7 @@
       <c r="R19" s="47"/>
       <c r="S19" s="47"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="47"/>
       <c r="B20" s="47"/>
       <c r="C20" s="47" t="s">
@@ -9986,7 +9987,7 @@
       <c r="R20" s="47"/>
       <c r="S20" s="47"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="47"/>
       <c r="B21" s="47"/>
       <c r="C21" s="47"/>
@@ -10009,7 +10010,7 @@
       <c r="R21" s="47"/>
       <c r="S21" s="47"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="47" t="s">
         <v>5</v>
       </c>
@@ -10040,7 +10041,7 @@
       <c r="R22" s="47"/>
       <c r="S22" s="47"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="47"/>
       <c r="B23" s="47"/>
       <c r="C23" s="47"/>
@@ -10101,28 +10102,28 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="46" customWidth="1"/>
-    <col min="2" max="2" width="22.6328125" style="46" customWidth="1"/>
-    <col min="3" max="3" width="40.81640625" style="46" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.54296875" style="46" customWidth="1"/>
-    <col min="5" max="5" width="25.90625" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" style="46" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="46" customWidth="1"/>
+    <col min="3" max="3" width="40.77734375" style="46" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" style="46" customWidth="1"/>
+    <col min="5" max="5" width="25.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="54" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="95" t="s">
+    <row r="1" spans="1:5" s="54" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="96" t="s">
         <v>457</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
         <v>0</v>
       </c>
@@ -10139,7 +10140,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>321</v>
       </c>
@@ -10152,7 +10153,7 @@
       <c r="D3" s="47"/>
       <c r="E3" s="47"/>
     </row>
-    <row r="4" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
         <v>321</v>
       </c>
@@ -10165,7 +10166,7 @@
       <c r="D4" s="47"/>
       <c r="E4" s="47"/>
     </row>
-    <row r="5" spans="1:5" s="46" customFormat="1" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="46" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
         <v>4</v>
       </c>
@@ -10191,25 +10192,25 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.36328125" style="46" customWidth="1"/>
-    <col min="3" max="3" width="26.08984375" style="46" customWidth="1"/>
-    <col min="4" max="4" width="20.08984375" style="46" customWidth="1"/>
-    <col min="6" max="6" width="28.6328125" style="46" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="46" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" style="46" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" style="46" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" style="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="54" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="112" t="s">
+    <row r="1" spans="1:6" s="54" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="113" t="s">
         <v>456</v>
       </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="114"/>
-    </row>
-    <row r="2" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="115"/>
+    </row>
+    <row r="2" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
@@ -10229,7 +10230,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>4</v>
       </c>
@@ -10239,7 +10240,7 @@
       <c r="E3" s="47"/>
       <c r="F3" s="47"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
         <v>5</v>
       </c>
@@ -10259,7 +10260,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="47"/>
       <c r="B5" s="47"/>
       <c r="C5" s="47"/>
@@ -10273,7 +10274,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="47"/>
       <c r="B6" s="47"/>
       <c r="C6" s="47" t="s">
@@ -10289,7 +10290,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
         <v>5</v>
       </c>
@@ -10330,40 +10331,40 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.54296875" style="46" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" style="46" customWidth="1"/>
-    <col min="4" max="4" width="17.90625" style="46" customWidth="1"/>
-    <col min="5" max="5" width="9.90625" style="46" customWidth="1"/>
-    <col min="7" max="7" width="11.81640625" style="46" customWidth="1"/>
-    <col min="8" max="8" width="12.453125" style="46" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" style="46" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" style="46" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" style="46" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" style="46" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" style="46" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" style="46" customWidth="1"/>
     <col min="9" max="9" width="15" style="46" customWidth="1"/>
-    <col min="12" max="12" width="10.1796875" style="46" customWidth="1"/>
-    <col min="16" max="16" width="11.6328125" customWidth="1"/>
+    <col min="12" max="12" width="10.21875" style="46" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="88.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="95" t="s">
+    <row r="1" spans="1:16" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="96" t="s">
         <v>484</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="95"/>
-      <c r="P1" s="95"/>
-    </row>
-    <row r="2" spans="1:16" ht="46.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="96"/>
+      <c r="O1" s="96"/>
+      <c r="P1" s="96"/>
+    </row>
+    <row r="2" spans="1:16" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
@@ -10413,7 +10414,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>4</v>
       </c>
@@ -10433,7 +10434,7 @@
       <c r="O3" s="47"/>
       <c r="P3" s="47"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
         <v>5</v>
       </c>
@@ -10475,7 +10476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="47"/>
       <c r="B5" s="47"/>
       <c r="C5" s="47" t="s">
@@ -10503,7 +10504,7 @@
       <c r="O5" s="47"/>
       <c r="P5" s="47"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>5</v>
       </c>
@@ -10562,17 +10563,17 @@
       <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="28.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.453125" style="46" customWidth="1"/>
-    <col min="2" max="2" width="35.08984375" style="46" customWidth="1"/>
-    <col min="3" max="3" width="19.1796875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.81640625" style="46" customWidth="1"/>
-    <col min="5" max="5" width="17.6328125" style="46" customWidth="1"/>
-    <col min="6" max="6" width="17.90625" style="46" customWidth="1"/>
+    <col min="1" max="1" width="35.44140625" style="46" customWidth="1"/>
+    <col min="2" max="2" width="35.109375" style="46" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.77734375" style="46" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="46" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" style="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>250</v>
       </c>
@@ -10592,7 +10593,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>215</v>
       </c>
@@ -10612,7 +10613,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
         <v>219</v>
       </c>
@@ -10632,7 +10633,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
         <v>199</v>
       </c>
@@ -10652,7 +10653,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>192</v>
       </c>
@@ -10670,7 +10671,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>212</v>
       </c>
@@ -10683,7 +10684,7 @@
       </c>
       <c r="F6" s="10"/>
     </row>
-    <row r="7" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>224</v>
       </c>
@@ -10692,7 +10693,7 @@
       </c>
       <c r="E7" s="10"/>
     </row>
-    <row r="8" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>198</v>
       </c>
@@ -10700,7 +10701,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>203</v>
       </c>
@@ -10708,7 +10709,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>217</v>
       </c>
@@ -10716,7 +10717,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>222</v>
       </c>
@@ -10724,153 +10725,153 @@
         <v>264</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19"/>
       <c r="B12" s="34" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="34" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="34" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="34" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="34" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="34" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="34" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="34" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="34" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="34" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="34" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="34" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="24" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="34" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="25" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="34" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="26" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="34" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="27" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="34" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="28" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="34" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="29" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="34" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="30" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="34" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="31" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="34" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="32" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="34" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="33" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="34" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="34" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="34" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="35" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="34" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="36" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="34" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="37" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="34" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="38" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="34" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="39" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="34" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="40" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="34" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="41" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="10"/>
     </row>
   </sheetData>
@@ -10887,34 +10888,34 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.90625" style="46" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" style="46" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="46" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.54296875" style="46" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.54296875" style="46" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.81640625" style="46" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.81640625" style="46" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.90625" style="46"/>
+    <col min="3" max="3" width="16.5546875" style="46" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" style="46" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" style="46" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" style="46" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="46"/>
     <col min="8" max="8" width="11" style="46" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.90625" style="46" customWidth="1"/>
-    <col min="10" max="16384" width="8.90625" style="46"/>
+    <col min="9" max="9" width="13.88671875" style="46" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="46"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="114" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="115" t="s">
+    <row r="1" spans="1:10" ht="114" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="116" t="s">
         <v>479</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="116"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -10943,7 +10944,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="64" t="s">
         <v>4</v>
       </c>
@@ -10956,7 +10957,7 @@
       <c r="H3" s="47"/>
       <c r="I3" s="47"/>
     </row>
-    <row r="4" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
         <v>321</v>
       </c>
@@ -10986,7 +10987,7 @@
       </c>
       <c r="J4" s="60"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
         <v>321</v>
       </c>
@@ -11031,60 +11032,60 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="20.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.1796875" style="46" customWidth="1"/>
+    <col min="1" max="1" width="10.21875" style="46" customWidth="1"/>
     <col min="2" max="2" width="14" style="46" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" style="46" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" style="46" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" style="46" customWidth="1"/>
-    <col min="6" max="6" width="14.08984375" style="46" customWidth="1"/>
-    <col min="7" max="7" width="11.453125" style="46" customWidth="1"/>
-    <col min="8" max="8" width="27.54296875" style="46" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" style="46" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="46" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" style="46" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="46" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" style="46" customWidth="1"/>
+    <col min="8" max="8" width="27.5546875" style="46" customWidth="1"/>
     <col min="9" max="9" width="13" style="46" customWidth="1"/>
-    <col min="10" max="10" width="16.54296875" style="46" customWidth="1"/>
-    <col min="11" max="11" width="14.36328125" style="68" customWidth="1"/>
-    <col min="12" max="13" width="20.54296875" style="46"/>
-    <col min="14" max="14" width="20.54296875" style="3"/>
-    <col min="15" max="17" width="20.54296875" style="46"/>
+    <col min="10" max="10" width="16.5546875" style="46" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" style="68" customWidth="1"/>
+    <col min="12" max="13" width="20.5546875" style="46"/>
+    <col min="14" max="14" width="20.5546875" style="3"/>
+    <col min="15" max="17" width="20.5546875" style="46"/>
     <col min="18" max="18" width="23" style="46" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="20.54296875" style="46"/>
-    <col min="22" max="22" width="23.1796875" style="46" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.1796875" style="46" customWidth="1"/>
-    <col min="24" max="24" width="20.54296875" style="46"/>
-    <col min="25" max="25" width="23.08984375" style="46" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="20.54296875" style="46"/>
+    <col min="19" max="21" width="20.5546875" style="46"/>
+    <col min="22" max="22" width="23.21875" style="46" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.21875" style="46" customWidth="1"/>
+    <col min="24" max="24" width="20.5546875" style="46"/>
+    <col min="25" max="25" width="23.109375" style="46" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="20.5546875" style="46"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="65" customFormat="1" ht="135.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="96" t="s">
+    <row r="1" spans="1:24" s="65" customFormat="1" ht="135.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="97" t="s">
         <v>604</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
-      <c r="M1" s="97"/>
-      <c r="N1" s="97"/>
-      <c r="O1" s="97"/>
-      <c r="P1" s="97"/>
-      <c r="Q1" s="97"/>
-      <c r="R1" s="97"/>
-      <c r="S1" s="97"/>
-      <c r="T1" s="97"/>
-      <c r="U1" s="97"/>
-      <c r="V1" s="97"/>
-      <c r="W1" s="97"/>
-      <c r="X1" s="98"/>
-    </row>
-    <row r="2" spans="1:24" s="81" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="98"/>
+      <c r="O1" s="98"/>
+      <c r="P1" s="98"/>
+      <c r="Q1" s="98"/>
+      <c r="R1" s="98"/>
+      <c r="S1" s="98"/>
+      <c r="T1" s="98"/>
+      <c r="U1" s="98"/>
+      <c r="V1" s="98"/>
+      <c r="W1" s="98"/>
+      <c r="X1" s="99"/>
+    </row>
+    <row r="2" spans="1:24" s="81" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="84" t="s">
         <v>0</v>
       </c>
@@ -11158,7 +11159,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="56" t="s">
         <v>4</v>
       </c>
@@ -11186,7 +11187,7 @@
       <c r="W3" s="47"/>
       <c r="X3" s="47"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="66" t="s">
         <v>321</v>
       </c>
@@ -11260,7 +11261,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="66" t="s">
         <v>321</v>
       </c>
@@ -11374,67 +11375,67 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.453125" style="46" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" style="46" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="46" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.90625" style="46" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.81640625" style="46" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1796875" style="46" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.90625" style="46" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.54296875" style="46" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.81640625" style="46" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.453125" style="46" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.54296875" style="46" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.81640625" style="68" customWidth="1"/>
-    <col min="12" max="12" width="14.81640625" style="46" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.90625" style="46" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.1796875" style="46" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.36328125" style="46" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.1796875" style="46" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.1796875" style="46" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" style="46" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.77734375" style="46" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" style="46" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" style="46" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" style="46" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.77734375" style="46" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" style="46" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5546875" style="46" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.77734375" style="68" customWidth="1"/>
+    <col min="12" max="12" width="14.77734375" style="46" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" style="46" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.21875" style="46" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.33203125" style="46" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.21875" style="46" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.21875" style="46" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="23" style="46" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.453125" style="46" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.90625" style="46" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.08984375" style="46" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="23.1796875" style="46" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.1796875" style="46" customWidth="1"/>
-    <col min="24" max="24" width="15.1796875" style="46" customWidth="1"/>
-    <col min="25" max="25" width="14.90625" style="46" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.44140625" style="46" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.88671875" style="46" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.109375" style="46" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.21875" style="46" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.21875" style="46" customWidth="1"/>
+    <col min="24" max="24" width="15.21875" style="46" customWidth="1"/>
+    <col min="25" max="25" width="14.88671875" style="46" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="42" style="46" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.1796875" style="46" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="8.81640625" style="46"/>
+    <col min="27" max="27" width="15.21875" style="46" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="8.77734375" style="46"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="65" customFormat="1" ht="133.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="96" t="s">
+    <row r="1" spans="1:24" s="65" customFormat="1" ht="133.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="97" t="s">
         <v>605</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
-      <c r="M1" s="97"/>
-      <c r="N1" s="97"/>
-      <c r="O1" s="97"/>
-      <c r="P1" s="97"/>
-      <c r="Q1" s="97"/>
-      <c r="R1" s="97"/>
-      <c r="S1" s="97"/>
-      <c r="T1" s="97"/>
-      <c r="U1" s="97"/>
-      <c r="V1" s="97"/>
-      <c r="W1" s="97"/>
-      <c r="X1" s="98"/>
-    </row>
-    <row r="2" spans="1:24" s="81" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="98"/>
+      <c r="O1" s="98"/>
+      <c r="P1" s="98"/>
+      <c r="Q1" s="98"/>
+      <c r="R1" s="98"/>
+      <c r="S1" s="98"/>
+      <c r="T1" s="98"/>
+      <c r="U1" s="98"/>
+      <c r="V1" s="98"/>
+      <c r="W1" s="98"/>
+      <c r="X1" s="99"/>
+    </row>
+    <row r="2" spans="1:24" s="81" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="84" t="s">
         <v>0</v>
       </c>
@@ -11508,7 +11509,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="56" t="s">
         <v>4</v>
       </c>
@@ -11536,7 +11537,7 @@
       <c r="W3" s="47"/>
       <c r="X3" s="47"/>
     </row>
-    <row r="4" spans="1:24" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="66" t="s">
         <v>321</v>
       </c>
@@ -11610,7 +11611,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="66" t="s">
         <v>321</v>
       </c>
@@ -11725,65 +11726,65 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.453125" style="46" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" style="46" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="46" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.81640625" style="46" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.1796875" style="46" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.54296875" style="46" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.54296875" style="46" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.453125" style="46" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.54296875" style="46" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.81640625" style="68" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.81640625" style="46" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.90625" style="46" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.1796875" style="46" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.36328125" style="46" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.1796875" style="46" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.1796875" style="46" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.77734375" style="46" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" style="46" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" style="46" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5546875" style="46" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" style="46" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5546875" style="46" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.77734375" style="68" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.77734375" style="46" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" style="46" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.21875" style="46" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.33203125" style="46" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.21875" style="46" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.21875" style="46" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="23" style="46" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.453125" style="46" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.90625" style="46" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.08984375" style="46" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="23.1796875" style="46" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.1796875" style="46" customWidth="1"/>
-    <col min="24" max="25" width="14.54296875" style="46" customWidth="1"/>
-    <col min="26" max="26" width="15.1796875" style="46" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="8.81640625" style="46"/>
+    <col min="19" max="19" width="13.44140625" style="46" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.88671875" style="46" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.109375" style="46" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.21875" style="46" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.21875" style="46" customWidth="1"/>
+    <col min="24" max="25" width="14.5546875" style="46" customWidth="1"/>
+    <col min="26" max="26" width="15.21875" style="46" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="8.77734375" style="46"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="65" customFormat="1" ht="195" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="96" t="s">
+    <row r="1" spans="1:24" s="65" customFormat="1" ht="195" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="97" t="s">
         <v>606</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
-      <c r="M1" s="97"/>
-      <c r="N1" s="97"/>
-      <c r="O1" s="97"/>
-      <c r="P1" s="97"/>
-      <c r="Q1" s="97"/>
-      <c r="R1" s="97"/>
-      <c r="S1" s="97"/>
-      <c r="T1" s="97"/>
-      <c r="U1" s="97"/>
-      <c r="V1" s="97"/>
-      <c r="W1" s="97"/>
-      <c r="X1" s="98"/>
-    </row>
-    <row r="2" spans="1:24" s="81" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="98"/>
+      <c r="O1" s="98"/>
+      <c r="P1" s="98"/>
+      <c r="Q1" s="98"/>
+      <c r="R1" s="98"/>
+      <c r="S1" s="98"/>
+      <c r="T1" s="98"/>
+      <c r="U1" s="98"/>
+      <c r="V1" s="98"/>
+      <c r="W1" s="98"/>
+      <c r="X1" s="99"/>
+    </row>
+    <row r="2" spans="1:24" s="81" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="84" t="s">
         <v>0</v>
       </c>
@@ -11857,7 +11858,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="75" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" s="75" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="72" t="s">
         <v>4</v>
       </c>
@@ -11884,7 +11885,7 @@
       <c r="W3" s="71"/>
       <c r="X3" s="64"/>
     </row>
-    <row r="4" spans="1:24" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="66" t="s">
         <v>5</v>
       </c>
@@ -11958,7 +11959,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="63"/>
       <c r="B5" s="60"/>
       <c r="C5" s="70"/>
@@ -12001,20 +12002,20 @@
       <selection activeCell="I2" sqref="I2:I108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.36328125" style="46" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" style="46" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42" style="46" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" style="46" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.1796875" style="46" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.90625" style="46" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.1796875" style="46" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.90625" style="46" customWidth="1"/>
-    <col min="9" max="9" width="15.90625" style="46" customWidth="1"/>
-    <col min="10" max="16384" width="8.90625" style="46"/>
+    <col min="3" max="3" width="9.77734375" style="46" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.21875" style="46" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" style="46" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.21875" style="46" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" style="46" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" style="46" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="46"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="61" t="s">
         <v>344</v>
       </c>
@@ -12043,7 +12044,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A2" s="47" t="s">
         <v>94</v>
       </c>
@@ -12072,7 +12073,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A3" s="47" t="s">
         <v>345</v>
       </c>
@@ -12101,7 +12102,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
         <v>346</v>
       </c>
@@ -12121,7 +12122,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
         <v>343</v>
       </c>
@@ -12141,7 +12142,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>347</v>
       </c>
@@ -12159,7 +12160,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
         <v>332</v>
       </c>
@@ -12177,7 +12178,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="47"/>
       <c r="B8" s="47"/>
       <c r="C8" s="47" t="s">
@@ -12193,7 +12194,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="47"/>
       <c r="B9" s="47"/>
       <c r="C9" s="47" t="s">
@@ -12209,7 +12210,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="47"/>
       <c r="B10" s="47"/>
       <c r="C10" s="47" t="s">
@@ -12225,7 +12226,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="47"/>
       <c r="B11" s="47"/>
       <c r="C11" s="47" t="s">
@@ -12241,7 +12242,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="47"/>
       <c r="B12" s="47"/>
       <c r="C12" s="47" t="s">
@@ -12255,7 +12256,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="47"/>
       <c r="B13" s="47"/>
       <c r="C13" s="47" t="s">
@@ -12269,7 +12270,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="47"/>
       <c r="B14" s="47"/>
       <c r="C14" s="47" t="s">
@@ -12283,472 +12284,472 @@
         <v>502</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I15" s="47" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I16" s="47" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I17" s="47" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I18" s="47" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I19" s="47" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I20" s="47" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="21" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I21" s="47" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I22" s="47" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I23" s="47" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="24" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I24" s="47" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="25" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I25" s="47" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="26" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I26" s="47" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="27" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I27" s="47" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="28" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I28" s="47" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="29" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I29" s="47" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="30" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I30" s="47" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="31" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I31" s="47" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="32" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I32" s="47" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="33" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I33" s="47" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="34" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I34" s="47" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="35" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I35" s="47" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="36" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I36" s="47" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="37" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I37" s="47" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="38" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I38" s="47" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="39" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I39" s="47" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="40" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I40" s="47" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="41" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I41" s="47" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="42" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I42" s="47" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="43" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I43" s="47" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="44" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I44" s="47" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="45" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I45" s="47" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="46" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I46" s="47" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="47" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I47" s="47" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="48" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I48" s="47" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I49" s="47" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I50" s="47" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I51" s="47" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I52" s="47" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="53" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I53" s="47" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="54" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I54" s="47" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="55" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I55" s="47" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="56" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I56" s="47" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="57" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I57" s="47" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="58" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I58" s="47" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="59" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I59" s="47" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="60" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I60" s="47" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="61" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I61" s="47" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="62" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I62" s="47" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="63" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I63" s="47" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="64" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I64" s="47" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="65" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I65" s="47" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="66" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I66" s="47" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="67" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I67" s="47" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="68" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I68" s="47" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="69" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I69" s="47" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="70" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I70" s="47" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="71" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I71" s="47" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="72" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I72" s="47" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="73" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I73" s="47" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="74" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I74" s="47" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="75" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I75" s="47" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="76" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I76" s="47" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="77" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I77" s="47" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="78" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I78" s="47" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="79" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I79" s="47" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="80" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I80" s="47" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="81" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I81" s="47" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="82" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I82" s="47" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="83" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I83" s="47" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="84" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I84" s="47" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="85" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I85" s="47" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="86" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I86" s="47" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="87" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I87" s="47" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="88" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I88" s="47" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="89" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I89" s="47" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="90" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I90" s="47" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="91" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I91" s="47" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="92" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I92" s="47" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="93" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I93" s="47" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="94" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I94" s="47" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="95" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I95" s="47" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="96" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I96" s="47" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="97" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I97" s="47" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="98" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I98" s="47" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="99" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I99" s="47" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="100" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I100" s="47" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="101" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I101" s="47" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="102" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I102" s="47" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="103" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I103" s="47" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="104" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I104" s="47" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="105" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I105" s="47" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="106" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I106" s="47" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="107" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I107" s="47" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="108" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I108" s="47" t="s">
         <v>596</v>
       </c>
@@ -12764,31 +12765,31 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="46" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" style="46" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" style="46" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="46" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32" style="46" customWidth="1"/>
-    <col min="4" max="4" width="31.36328125" customWidth="1"/>
-    <col min="5" max="5" width="24.453125" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="54" customFormat="1" ht="105.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="95" t="s">
+    <row r="1" spans="1:5" s="54" customFormat="1" ht="105.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="96" t="s">
         <v>458</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -12805,7 +12806,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>321</v>
       </c>
@@ -12818,7 +12819,7 @@
       <c r="D3" s="47"/>
       <c r="E3" s="47"/>
     </row>
-    <row r="4" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
         <v>321</v>
       </c>
@@ -12831,7 +12832,7 @@
       <c r="D4" s="47"/>
       <c r="E4" s="47"/>
     </row>
-    <row r="5" spans="1:5" s="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
         <v>321</v>
       </c>
@@ -12844,7 +12845,7 @@
       <c r="D5" s="47"/>
       <c r="E5" s="47"/>
     </row>
-    <row r="6" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>321</v>
       </c>
@@ -12857,8 +12858,8 @@
       <c r="D6" s="47"/>
       <c r="E6" s="47"/>
     </row>
-    <row r="7" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="47" t="s">
+    <row r="7" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="25" t="s">
         <v>321</v>
       </c>
       <c r="B7" s="25" t="s">
@@ -12870,7 +12871,7 @@
       <c r="D7" s="25"/>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" s="47" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" s="60" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="47" t="s">
         <v>321</v>
       </c>
@@ -12883,7 +12884,7 @@
       <c r="D8" s="45"/>
       <c r="E8" s="45"/>
     </row>
-    <row r="9" spans="1:5" s="47" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="47" t="s">
         <v>321</v>
       </c>
@@ -12893,8 +12894,10 @@
       <c r="C9" s="45" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+    </row>
+    <row r="10" spans="1:5" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="47" t="s">
         <v>321</v>
       </c>
@@ -12904,8 +12907,10 @@
       <c r="C10" s="45" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+    </row>
+    <row r="11" spans="1:5" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="47" t="s">
         <v>321</v>
       </c>
@@ -12915,8 +12920,10 @@
       <c r="C11" s="45" t="s">
         <v>645</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+    </row>
+    <row r="12" spans="1:5" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="47" t="s">
         <v>321</v>
       </c>
@@ -12926,19 +12933,23 @@
       <c r="C12" s="45" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="47" t="s">
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+    </row>
+    <row r="13" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
         <v>321</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="95" t="s">
         <v>648</v>
       </c>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="24" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+    </row>
+    <row r="14" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="47" t="s">
         <v>321</v>
       </c>
@@ -12948,8 +12959,10 @@
       <c r="C14" s="45" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+    </row>
+    <row r="15" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="47" t="s">
         <v>321</v>
       </c>
@@ -12959,6 +12972,17 @@
       <c r="C15" s="45" t="s">
         <v>652</v>
       </c>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="47"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -12976,34 +13000,34 @@
   </sheetPr>
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="46" customWidth="1"/>
-    <col min="2" max="2" width="17.08984375" style="46" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.36328125" style="46" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" style="46" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" style="46" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" style="46" customWidth="1"/>
     <col min="4" max="4" width="16" style="46" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.36328125" style="46" customWidth="1"/>
-    <col min="6" max="7" width="28.453125" style="46" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.6328125" customWidth="1"/>
+    <col min="5" max="5" width="49.33203125" style="46" customWidth="1"/>
+    <col min="6" max="7" width="28.44140625" style="46" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="54" customFormat="1" ht="102.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="95" t="s">
+    <row r="1" spans="1:8" s="54" customFormat="1" ht="102.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="96" t="s">
         <v>459</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-    </row>
-    <row r="2" spans="1:8" s="54" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+    </row>
+    <row r="2" spans="1:8" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -13029,7 +13053,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="46" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" s="46" customFormat="1" ht="52.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>321</v>
       </c>
@@ -13049,7 +13073,7 @@
       <c r="G3" s="45"/>
       <c r="H3" s="94"/>
     </row>
-    <row r="4" spans="1:8" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
         <v>321</v>
       </c>
@@ -13067,8 +13091,9 @@
       </c>
       <c r="F4" s="47"/>
       <c r="G4" s="47"/>
-    </row>
-    <row r="5" spans="1:8" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H4" s="47"/>
+    </row>
+    <row r="5" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
         <v>321</v>
       </c>
@@ -13086,8 +13111,9 @@
       </c>
       <c r="F5" s="47"/>
       <c r="G5" s="47"/>
-    </row>
-    <row r="6" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="H5" s="47"/>
+    </row>
+    <row r="6" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="47"/>
       <c r="B6" s="45"/>
       <c r="C6" s="47"/>
@@ -13097,8 +13123,9 @@
       </c>
       <c r="F6" s="47"/>
       <c r="G6" s="47"/>
-    </row>
-    <row r="7" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="H6" s="47"/>
+    </row>
+    <row r="7" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="47"/>
       <c r="B7" s="45"/>
       <c r="C7" s="47"/>
@@ -13108,8 +13135,9 @@
       </c>
       <c r="F7" s="47"/>
       <c r="G7" s="47"/>
-    </row>
-    <row r="8" spans="1:8" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H7" s="47"/>
+    </row>
+    <row r="8" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="47"/>
       <c r="B8" s="45"/>
       <c r="C8" s="47"/>
@@ -13119,8 +13147,9 @@
       </c>
       <c r="F8" s="47"/>
       <c r="G8" s="47"/>
-    </row>
-    <row r="9" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="H8" s="47"/>
+    </row>
+    <row r="9" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="47"/>
       <c r="B9" s="45"/>
       <c r="C9" s="47"/>
@@ -13130,8 +13159,9 @@
       </c>
       <c r="F9" s="47"/>
       <c r="G9" s="47"/>
-    </row>
-    <row r="10" spans="1:8" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H9" s="47"/>
+    </row>
+    <row r="10" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="47"/>
       <c r="B10" s="45"/>
       <c r="C10" s="47"/>
@@ -13141,8 +13171,9 @@
       </c>
       <c r="F10" s="47"/>
       <c r="G10" s="47"/>
-    </row>
-    <row r="11" spans="1:8" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H10" s="47"/>
+    </row>
+    <row r="11" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="47"/>
       <c r="B11" s="45"/>
       <c r="C11" s="47"/>
@@ -13152,8 +13183,9 @@
       </c>
       <c r="F11" s="47"/>
       <c r="G11" s="47"/>
-    </row>
-    <row r="12" spans="1:8" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H11" s="47"/>
+    </row>
+    <row r="12" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="47" t="s">
         <v>321</v>
       </c>
@@ -13171,8 +13203,9 @@
       </c>
       <c r="F12" s="47"/>
       <c r="G12" s="47"/>
-    </row>
-    <row r="13" spans="1:8" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H12" s="47"/>
+    </row>
+    <row r="13" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="47" t="s">
         <v>321</v>
       </c>
@@ -13190,8 +13223,9 @@
       </c>
       <c r="F13" s="47"/>
       <c r="G13" s="47"/>
-    </row>
-    <row r="14" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="H13" s="47"/>
+    </row>
+    <row r="14" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="47"/>
       <c r="B14" s="45"/>
       <c r="C14" s="47"/>
@@ -13201,8 +13235,9 @@
       </c>
       <c r="F14" s="47"/>
       <c r="G14" s="47"/>
-    </row>
-    <row r="15" spans="1:8" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H14" s="47"/>
+    </row>
+    <row r="15" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="47"/>
       <c r="B15" s="45"/>
       <c r="C15" s="47"/>
@@ -13212,8 +13247,9 @@
       </c>
       <c r="F15" s="47"/>
       <c r="G15" s="47"/>
-    </row>
-    <row r="16" spans="1:8" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H15" s="47"/>
+    </row>
+    <row r="16" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="47"/>
       <c r="B16" s="45"/>
       <c r="C16" s="47"/>
@@ -13223,8 +13259,9 @@
       </c>
       <c r="F16" s="47"/>
       <c r="G16" s="47"/>
-    </row>
-    <row r="17" spans="1:7" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H16" s="47"/>
+    </row>
+    <row r="17" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="47" t="s">
         <v>321</v>
       </c>
@@ -13242,8 +13279,9 @@
       </c>
       <c r="F17" s="47"/>
       <c r="G17" s="47"/>
-    </row>
-    <row r="18" spans="1:7" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H17" s="47"/>
+    </row>
+    <row r="18" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="47"/>
       <c r="B18" s="45"/>
       <c r="C18" s="47"/>
@@ -13253,8 +13291,9 @@
       </c>
       <c r="F18" s="47"/>
       <c r="G18" s="47"/>
-    </row>
-    <row r="19" spans="1:7" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H18" s="47"/>
+    </row>
+    <row r="19" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="47"/>
       <c r="B19" s="45"/>
       <c r="C19" s="47"/>
@@ -13264,8 +13303,9 @@
       </c>
       <c r="F19" s="47"/>
       <c r="G19" s="47"/>
-    </row>
-    <row r="20" spans="1:7" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H19" s="47"/>
+    </row>
+    <row r="20" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="47"/>
       <c r="B20" s="45"/>
       <c r="C20" s="47"/>
@@ -13275,8 +13315,9 @@
       </c>
       <c r="F20" s="47"/>
       <c r="G20" s="47"/>
-    </row>
-    <row r="21" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="H20" s="47"/>
+    </row>
+    <row r="21" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="47"/>
       <c r="B21" s="45"/>
       <c r="C21" s="47"/>
@@ -13286,8 +13327,9 @@
       </c>
       <c r="F21" s="47"/>
       <c r="G21" s="47"/>
-    </row>
-    <row r="22" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="H21" s="47"/>
+    </row>
+    <row r="22" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="47"/>
       <c r="B22" s="45"/>
       <c r="C22" s="47"/>
@@ -13297,8 +13339,9 @@
       </c>
       <c r="F22" s="47"/>
       <c r="G22" s="47"/>
-    </row>
-    <row r="23" spans="1:7" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H22" s="47"/>
+    </row>
+    <row r="23" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="47"/>
       <c r="B23" s="45"/>
       <c r="C23" s="47"/>
@@ -13308,8 +13351,9 @@
       </c>
       <c r="F23" s="47"/>
       <c r="G23" s="47"/>
-    </row>
-    <row r="24" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="H23" s="47"/>
+    </row>
+    <row r="24" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="47"/>
       <c r="B24" s="45"/>
       <c r="C24" s="47"/>
@@ -13319,8 +13363,9 @@
       </c>
       <c r="F24" s="47"/>
       <c r="G24" s="47"/>
-    </row>
-    <row r="25" spans="1:7" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H24" s="47"/>
+    </row>
+    <row r="25" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="47"/>
       <c r="B25" s="45"/>
       <c r="C25" s="47"/>
@@ -13330,8 +13375,9 @@
       </c>
       <c r="F25" s="47"/>
       <c r="G25" s="47"/>
-    </row>
-    <row r="26" spans="1:7" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H25" s="47"/>
+    </row>
+    <row r="26" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="47" t="s">
         <v>321</v>
       </c>
@@ -13349,8 +13395,9 @@
       </c>
       <c r="F26" s="47"/>
       <c r="G26" s="47"/>
-    </row>
-    <row r="27" spans="1:7" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H26" s="47"/>
+    </row>
+    <row r="27" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="47"/>
       <c r="B27" s="45"/>
       <c r="C27" s="47"/>
@@ -13360,8 +13407,9 @@
       </c>
       <c r="F27" s="47"/>
       <c r="G27" s="47"/>
-    </row>
-    <row r="28" spans="1:7" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H27" s="47"/>
+    </row>
+    <row r="28" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="47"/>
       <c r="B28" s="45"/>
       <c r="C28" s="47"/>
@@ -13371,8 +13419,9 @@
       </c>
       <c r="F28" s="47"/>
       <c r="G28" s="47"/>
-    </row>
-    <row r="29" spans="1:7" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H28" s="47"/>
+    </row>
+    <row r="29" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="47"/>
       <c r="B29" s="45"/>
       <c r="C29" s="47"/>
@@ -13382,8 +13431,9 @@
       </c>
       <c r="F29" s="47"/>
       <c r="G29" s="47"/>
-    </row>
-    <row r="30" spans="1:7" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H29" s="47"/>
+    </row>
+    <row r="30" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="47" t="s">
         <v>321</v>
       </c>
@@ -13401,8 +13451,9 @@
       </c>
       <c r="F30" s="47"/>
       <c r="G30" s="47"/>
-    </row>
-    <row r="31" spans="1:7" s="46" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="H30" s="47"/>
+    </row>
+    <row r="31" spans="1:8" s="46" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="47"/>
       <c r="B31" s="45"/>
       <c r="C31" s="47"/>
@@ -13412,8 +13463,9 @@
       </c>
       <c r="F31" s="47"/>
       <c r="G31" s="47"/>
-    </row>
-    <row r="32" spans="1:7" s="46" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="H31" s="47"/>
+    </row>
+    <row r="32" spans="1:8" s="46" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="47"/>
       <c r="B32" s="45"/>
       <c r="C32" s="47"/>
@@ -13423,8 +13475,9 @@
       </c>
       <c r="F32" s="47"/>
       <c r="G32" s="47"/>
-    </row>
-    <row r="33" spans="1:7" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H32" s="47"/>
+    </row>
+    <row r="33" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="47"/>
       <c r="B33" s="45"/>
       <c r="C33" s="47"/>
@@ -13434,8 +13487,9 @@
       </c>
       <c r="F33" s="47"/>
       <c r="G33" s="47"/>
-    </row>
-    <row r="34" spans="1:7" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H33" s="47"/>
+    </row>
+    <row r="34" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="47"/>
       <c r="B34" s="45"/>
       <c r="C34" s="47"/>
@@ -13445,8 +13499,9 @@
       </c>
       <c r="F34" s="47"/>
       <c r="G34" s="47"/>
-    </row>
-    <row r="35" spans="1:7" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H34" s="47"/>
+    </row>
+    <row r="35" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="47"/>
       <c r="B35" s="45"/>
       <c r="C35" s="47"/>
@@ -13456,8 +13511,9 @@
       </c>
       <c r="F35" s="47"/>
       <c r="G35" s="47"/>
-    </row>
-    <row r="36" spans="1:7" s="46" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="H35" s="47"/>
+    </row>
+    <row r="36" spans="1:8" s="46" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="47" t="s">
         <v>321</v>
       </c>
@@ -13475,8 +13531,9 @@
       </c>
       <c r="F36" s="47"/>
       <c r="G36" s="47"/>
-    </row>
-    <row r="37" spans="1:7" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H36" s="47"/>
+    </row>
+    <row r="37" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="47"/>
       <c r="B37" s="45"/>
       <c r="C37" s="47"/>
@@ -13486,8 +13543,9 @@
       </c>
       <c r="F37" s="47"/>
       <c r="G37" s="47"/>
-    </row>
-    <row r="38" spans="1:7" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H37" s="47"/>
+    </row>
+    <row r="38" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="47"/>
       <c r="B38" s="45"/>
       <c r="C38" s="47"/>
@@ -13497,8 +13555,9 @@
       </c>
       <c r="F38" s="47"/>
       <c r="G38" s="47"/>
-    </row>
-    <row r="39" spans="1:7" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H38" s="47"/>
+    </row>
+    <row r="39" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="47"/>
       <c r="B39" s="45"/>
       <c r="C39" s="47"/>
@@ -13508,8 +13567,9 @@
       </c>
       <c r="F39" s="47"/>
       <c r="G39" s="47"/>
-    </row>
-    <row r="40" spans="1:7" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H39" s="47"/>
+    </row>
+    <row r="40" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="47"/>
       <c r="B40" s="45"/>
       <c r="C40" s="47"/>
@@ -13519,8 +13579,9 @@
       </c>
       <c r="F40" s="47"/>
       <c r="G40" s="47"/>
-    </row>
-    <row r="41" spans="1:7" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H40" s="47"/>
+    </row>
+    <row r="41" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="47" t="s">
         <v>321</v>
       </c>
@@ -13538,8 +13599,9 @@
       </c>
       <c r="F41" s="47"/>
       <c r="G41" s="47"/>
-    </row>
-    <row r="42" spans="1:7" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H41" s="47"/>
+    </row>
+    <row r="42" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="47" t="s">
         <v>321</v>
       </c>
@@ -13557,8 +13619,9 @@
       </c>
       <c r="F42" s="47"/>
       <c r="G42" s="47"/>
-    </row>
-    <row r="43" spans="1:7" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H42" s="47"/>
+    </row>
+    <row r="43" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="47"/>
       <c r="B43" s="45"/>
       <c r="C43" s="47"/>
@@ -13568,8 +13631,9 @@
       </c>
       <c r="F43" s="47"/>
       <c r="G43" s="47"/>
-    </row>
-    <row r="44" spans="1:7" s="46" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H43" s="47"/>
+    </row>
+    <row r="44" spans="1:8" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="47" t="s">
         <v>321</v>
       </c>
@@ -13587,8 +13651,9 @@
       </c>
       <c r="F44" s="47"/>
       <c r="G44" s="47"/>
-    </row>
-    <row r="45" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="H44" s="47"/>
+    </row>
+    <row r="45" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="47" t="s">
         <v>4</v>
       </c>
@@ -13598,6 +13663,7 @@
       <c r="E45" s="45"/>
       <c r="F45" s="47"/>
       <c r="G45" s="47"/>
+      <c r="H45" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -13615,37 +13681,37 @@
       <selection activeCell="A3" sqref="A3:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="4"/>
-    <col min="2" max="2" width="19.1796875" style="46" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" style="46" customWidth="1"/>
-    <col min="4" max="4" width="20.36328125" style="46" customWidth="1"/>
-    <col min="5" max="5" width="9.90625" style="46" customWidth="1"/>
-    <col min="6" max="6" width="21.90625" style="46" customWidth="1"/>
-    <col min="7" max="7" width="21.6328125" style="46" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="4"/>
+    <col min="2" max="2" width="19.21875" style="46" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" style="46" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="46" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" style="46" customWidth="1"/>
+    <col min="6" max="6" width="21.88671875" style="46" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" style="46" customWidth="1"/>
     <col min="8" max="8" width="21" style="46" customWidth="1"/>
-    <col min="9" max="9" width="23.81640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="18.6328125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="23.77734375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="131.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="96" t="s">
+    <row r="1" spans="1:10" ht="131.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="97" t="s">
         <v>490</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="99" t="s">
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="100" t="s">
         <v>487</v>
       </c>
-      <c r="H1" s="100"/>
-      <c r="I1" s="100"/>
-      <c r="J1" s="101"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H1" s="101"/>
+      <c r="I1" s="101"/>
+      <c r="J1" s="102"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="51" t="s">
         <v>0</v>
       </c>
@@ -13677,7 +13743,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="53" t="s">
         <v>4</v>
       </c>
@@ -13691,7 +13757,7 @@
       <c r="I3" s="52"/>
       <c r="J3" s="53"/>
     </row>
-    <row r="4" spans="1:10" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="59" t="s">
         <v>5</v>
       </c>
@@ -13721,7 +13787,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="59"/>
       <c r="B5" s="35"/>
       <c r="C5" s="36"/>
@@ -13741,7 +13807,7 @@
       </c>
       <c r="J5" s="38"/>
     </row>
-    <row r="6" spans="1:10" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="59" t="s">
         <v>5</v>
       </c>
@@ -13761,7 +13827,7 @@
       <c r="I6" s="59"/>
       <c r="J6" s="38"/>
     </row>
-    <row r="7" spans="1:10" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="59" t="s">
         <v>5</v>
       </c>
@@ -13783,7 +13849,7 @@
       <c r="I7" s="33"/>
       <c r="J7" s="38"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="59"/>
       <c r="B8" s="35"/>
       <c r="C8" s="36"/>
@@ -13797,7 +13863,7 @@
       <c r="I8" s="37"/>
       <c r="J8" s="38"/>
     </row>
-    <row r="9" spans="1:10" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="59" t="s">
         <v>5</v>
       </c>
@@ -13825,7 +13891,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="38"/>
       <c r="B10" s="35"/>
       <c r="C10" s="36"/>
@@ -13839,7 +13905,7 @@
       <c r="I10" s="37"/>
       <c r="J10" s="38"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="59"/>
       <c r="B11" s="35"/>
       <c r="C11" s="39"/>
@@ -13853,7 +13919,7 @@
       <c r="I11" s="37"/>
       <c r="J11" s="38"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="59"/>
       <c r="B12" s="35"/>
       <c r="C12" s="39"/>
@@ -13890,40 +13956,40 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="46" customWidth="1"/>
-    <col min="2" max="3" width="16.453125" style="46" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" style="46" customWidth="1"/>
-    <col min="5" max="5" width="13.6328125" style="46" customWidth="1"/>
-    <col min="6" max="6" width="21.54296875" style="46" customWidth="1"/>
-    <col min="7" max="7" width="14.36328125" style="46" customWidth="1"/>
-    <col min="8" max="8" width="14.453125" style="46" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" style="46" customWidth="1"/>
+    <col min="2" max="3" width="16.44140625" style="46" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" style="46" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="46" customWidth="1"/>
+    <col min="6" max="6" width="21.5546875" style="46" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="46" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" style="46" customWidth="1"/>
     <col min="9" max="9" width="14" style="46" customWidth="1"/>
-    <col min="10" max="10" width="22.54296875" style="46" customWidth="1"/>
-    <col min="11" max="11" width="26.453125" style="46" customWidth="1"/>
+    <col min="10" max="10" width="22.5546875" style="46" customWidth="1"/>
+    <col min="11" max="11" width="26.44140625" style="46" customWidth="1"/>
     <col min="12" max="12" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="46" customFormat="1" ht="187.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="96" t="s">
+    <row r="1" spans="1:12" s="46" customFormat="1" ht="187.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="97" t="s">
         <v>473</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="96" t="s">
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="97" t="s">
         <v>474</v>
       </c>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="98"/>
-    </row>
-    <row r="2" spans="1:12" s="54" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="99"/>
+    </row>
+    <row r="2" spans="1:12" s="54" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -13961,7 +14027,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="43" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" s="43" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>321</v>
       </c>
@@ -13995,7 +14061,7 @@
       <c r="K3" s="47"/>
       <c r="L3" s="42"/>
     </row>
-    <row r="4" spans="1:12" s="46" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" s="46" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="42" t="s">
         <v>4</v>
       </c>
@@ -14032,21 +14098,21 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.1796875" style="46" customWidth="1"/>
-    <col min="2" max="2" width="50.54296875" style="46" customWidth="1"/>
-    <col min="3" max="10" width="9.1796875" style="46" customWidth="1"/>
-    <col min="11" max="16384" width="9.1796875" style="46"/>
+    <col min="1" max="1" width="32.21875" style="46" customWidth="1"/>
+    <col min="2" max="2" width="50.5546875" style="46" customWidth="1"/>
+    <col min="3" max="10" width="9.21875" style="46" customWidth="1"/>
+    <col min="11" max="16384" width="9.21875" style="46"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="54" customFormat="1" ht="121.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="95" t="s">
+    <row r="1" spans="1:2" s="54" customFormat="1" ht="121.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="96" t="s">
         <v>453</v>
       </c>
-      <c r="B1" s="101"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B1" s="102"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>23</v>
       </c>
@@ -14054,13 +14120,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="47"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
@@ -14068,7 +14134,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -14076,7 +14142,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
@@ -14104,31 +14170,31 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="46" customWidth="1"/>
-    <col min="2" max="2" width="27.453125" style="46" customWidth="1"/>
-    <col min="3" max="3" width="17.1796875" style="46" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" style="46" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.453125" style="46" customWidth="1"/>
-    <col min="6" max="6" width="17.81640625" style="46" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.54296875" style="46" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" style="46" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" style="46" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" style="46" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" style="46" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" style="46" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" style="46" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.5546875" style="46" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="103.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="95" t="s">
+    <row r="1" spans="1:8" ht="103.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="96" t="s">
         <v>460</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-    </row>
-    <row r="2" spans="1:8" s="54" customFormat="1" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+    </row>
+    <row r="2" spans="1:8" s="54" customFormat="1" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -14154,7 +14220,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>4</v>
       </c>
@@ -14186,52 +14252,52 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="46" customWidth="1"/>
-    <col min="2" max="2" width="18.90625" style="46" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" style="46" customWidth="1"/>
-    <col min="4" max="4" width="19.1796875" style="46" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" style="46" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.1796875" style="46" customWidth="1"/>
-    <col min="7" max="7" width="18.1796875" style="46" customWidth="1"/>
-    <col min="8" max="8" width="18.453125" style="46" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="18.453125" style="46" customWidth="1"/>
-    <col min="11" max="11" width="11.36328125" style="46" customWidth="1"/>
-    <col min="12" max="12" width="14.36328125" style="46" customWidth="1"/>
-    <col min="13" max="13" width="15.81640625" style="46" customWidth="1"/>
-    <col min="14" max="14" width="13.6328125" style="46" customWidth="1"/>
-    <col min="15" max="15" width="11.90625" style="46" customWidth="1"/>
-    <col min="16" max="16" width="14.08984375" style="46" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" style="46" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" style="46" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" style="46" customWidth="1"/>
+    <col min="4" max="4" width="19.21875" style="46" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" style="46" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.21875" style="46" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" style="46" customWidth="1"/>
+    <col min="8" max="8" width="18.44140625" style="46" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="18.44140625" style="46" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" style="46" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" style="46" customWidth="1"/>
+    <col min="13" max="13" width="15.77734375" style="46" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" style="46" customWidth="1"/>
+    <col min="15" max="15" width="11.88671875" style="46" customWidth="1"/>
+    <col min="16" max="16" width="14.109375" style="46" customWidth="1"/>
     <col min="17" max="17" width="10" style="46" customWidth="1"/>
-    <col min="18" max="18" width="24.1796875" customWidth="1"/>
+    <col min="18" max="18" width="24.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="173.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="96" t="s">
+    <row r="1" spans="1:18" ht="173.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="97" t="s">
         <v>454</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="102" t="s">
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="103" t="s">
         <v>461</v>
       </c>
-      <c r="J1" s="102"/>
-      <c r="K1" s="102"/>
-      <c r="L1" s="102"/>
-      <c r="M1" s="102"/>
-      <c r="N1" s="102"/>
-      <c r="O1" s="102"/>
-      <c r="P1" s="102"/>
-      <c r="Q1" s="102"/>
-      <c r="R1" s="102"/>
-    </row>
-    <row r="2" spans="1:18" s="54" customFormat="1" ht="59.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="103"/>
+      <c r="N1" s="103"/>
+      <c r="O1" s="103"/>
+      <c r="P1" s="103"/>
+      <c r="Q1" s="103"/>
+      <c r="R1" s="103"/>
+    </row>
+    <row r="2" spans="1:18" s="54" customFormat="1" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -14287,7 +14353,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="46" t="s">
         <v>5</v>
       </c>
@@ -14333,7 +14399,7 @@
       <c r="Q3" s="58"/>
       <c r="R3" s="42"/>
     </row>
-    <row r="4" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="46" t="s">
         <v>5</v>
       </c>
@@ -14379,7 +14445,7 @@
       <c r="Q4" s="58"/>
       <c r="R4" s="47"/>
     </row>
-    <row r="5" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="46" t="s">
         <v>5</v>
       </c>
@@ -14425,7 +14491,7 @@
       <c r="Q5" s="58"/>
       <c r="R5" s="47"/>
     </row>
-    <row r="6" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>4</v>
       </c>

</xml_diff>